<commit_message>
Added EventId in Second Position
</commit_message>
<xml_diff>
--- a/downloadfile/appointment.xlsx
+++ b/downloadfile/appointment.xlsx
@@ -25,6 +25,9 @@
     <t xml:space="preserve">COID</t>
   </si>
   <si>
+    <t xml:space="preserve">EventId</t>
+  </si>
+  <si>
     <t xml:space="preserve">Re-Sign Appt Date Text</t>
   </si>
   <si>
@@ -32,9 +35,6 @@
   </si>
   <si>
     <t xml:space="preserve">Company Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EventId</t>
   </si>
 </sst>
 </file>
@@ -153,8 +153,12 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <dxfs count="2">
-    <dxf/>
-    <dxf/>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+    </dxf>
   </dxfs>
 </styleSheet>
 </file>
@@ -164,47 +168,45 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.68"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="25.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1">
+  <conditionalFormatting sqref="D1">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1">
+  <conditionalFormatting sqref="D1">
     <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>0</formula>
     </cfRule>

</xml_diff>